<commit_message>
modify the made data. To be modified...
</commit_message>
<xml_diff>
--- a/判断矩阵权重计算.xlsx
+++ b/判断矩阵权重计算.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>W</t>
   </si>
@@ -146,14 +146,26 @@
     <t>cr总</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t>组合权重及总排序</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>因素</t>
+  </si>
+  <si>
+    <t>组合权重</t>
+  </si>
+  <si>
+    <t>总排序</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="178" formatCode="0.0000_);[Red]\(0.0000\)"/>
-    <numFmt numFmtId="179" formatCode="0.0000000_);[Red]\(0.0000000\)"/>
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -251,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -284,11 +296,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -299,6 +310,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3045,6 +3062,640 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="图片 53"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11591925" y="1200150"/>
+          <a:ext cx="161925" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="图片 54"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12277725" y="1200150"/>
+          <a:ext cx="161925" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="图片 55"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12963525" y="1200150"/>
+          <a:ext cx="161925" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="图片 56"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10906125" y="1419225"/>
+          <a:ext cx="161925" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="图片 57"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10906125" y="1638300"/>
+          <a:ext cx="161925" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="图片 58"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10906125" y="1838325"/>
+          <a:ext cx="161925" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="图片 59"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10906125" y="2038350"/>
+          <a:ext cx="152400" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="图片 67"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10906125" y="2238375"/>
+          <a:ext cx="161925" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="图片 69"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10906125" y="2438400"/>
+          <a:ext cx="161925" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="914400" cy="266611"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7600950" y="9415462"/>
+          <a:ext cx="914400" cy="266611"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3335,10 +3986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N65"/>
+  <dimension ref="A1:T65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47:H52"/>
+      <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3354,7 +4005,7 @@
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -3372,7 +4023,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3388,14 +4039,14 @@
       </c>
       <c r="M2" s="12">
         <f>L27*E6+I42*E7+L65*E8</f>
-        <v>5.8762186794134981E-2</v>
+        <v>2.6350369765900963E-2</v>
       </c>
       <c r="N2" s="12">
         <f>M2/L2</f>
-        <v>4.9468551526851312E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
+        <v>2.2182881469042941E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A3" s="9"/>
       <c r="B3" s="1">
         <v>1</v>
@@ -3411,7 +4062,7 @@
         <v>0.14347826086956519</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="4">
         <f>1/C3</f>
@@ -3428,13 +4079,13 @@
         <v>7.898550724637679E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <f>1/D3</f>
         <v>6</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <f>1/D4</f>
         <v>9</v>
       </c>
@@ -3452,7 +4103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="12">
         <f>B3/(B3+B4+B5)</f>
         <v>0.13333333333333333</v>
@@ -3469,7 +4120,7 @@
         <f>1/3*(B6+C6+D6)</f>
         <v>0.14347826086956519</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="12">
         <f t="array" ref="F6:F8">MMULT(B3:D5,E6:E8)</f>
         <v>0.43103864734299513</v>
       </c>
@@ -3477,8 +4128,11 @@
         <f>F6/E6</f>
         <v>3.0042087542087543</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12">
         <f>B4/(B4+B5+B3)</f>
         <v>6.6666666666666666E-2</v>
@@ -3495,15 +4149,27 @@
         <f t="shared" ref="E7:E8" si="1">1/3*(B7+C7+D7)</f>
         <v>7.898550724637679E-2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="12">
         <v>0.23711755233494358</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" ref="G7:G8" si="2">F7/E7</f>
         <v>3.0020387359836902</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
         <f>B5/(B5+B4+B3)</f>
         <v>0.8</v>
@@ -3520,7 +4186,7 @@
         <f t="shared" si="1"/>
         <v>0.77753623188405785</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="12">
         <v>2.3492753623188403</v>
       </c>
       <c r="G8" s="3">
@@ -3536,17 +4202,42 @@
       <c r="J8" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O8" s="18"/>
+      <c r="P8" s="12">
+        <f>H21</f>
+        <v>0.27737594649359354</v>
+      </c>
+      <c r="Q8" s="12">
+        <f>E39</f>
+        <v>0.12218196457326892</v>
+      </c>
+      <c r="R8" s="12">
+        <f>H59</f>
+        <v>3.3405366386780107E-2</v>
+      </c>
+      <c r="S8" s="12">
+        <f t="array" ref="S8:S13">MMULT(P8:R13,E6:E8)</f>
+        <v>7.5421905563212224E-2</v>
+      </c>
+      <c r="T8" s="3">
+        <f>RANK(S8,$S$8:$S$13)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="E9" s="3">
+        <f>SUM(E6:E8)</f>
+        <v>0.99999999999999978</v>
+      </c>
       <c r="G9" s="3">
         <f>SUM(G6:G8)</f>
         <v>9.0276827185242254</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="12">
         <f>G9/3</f>
         <v>3.0092275728414086</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="12">
         <f>(H9-3)/2</f>
         <v>4.6137864207043133E-3</v>
       </c>
@@ -3554,208 +4245,313 @@
         <f>I9/0.58</f>
         <v>7.9548041736281268E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O9" s="10"/>
+      <c r="P9" s="12">
+        <f t="shared" ref="P9:P13" si="3">H22</f>
+        <v>0.47514816338345756</v>
+      </c>
+      <c r="Q9" s="12">
+        <f>E40</f>
+        <v>0.2298711755233494</v>
+      </c>
+      <c r="R9" s="12">
+        <f t="shared" ref="R9:R13" si="4">H60</f>
+        <v>0.1624516557469915</v>
+      </c>
+      <c r="S9" s="12">
+        <v>0.2126419718105011</v>
+      </c>
+      <c r="T9" s="3">
+        <f t="shared" ref="T9:T13" si="5">RANK(S9,$S$8:$S$13)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="H10" s="12"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="12">
+        <f t="shared" si="3"/>
+        <v>5.4332795019069527E-2</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0</v>
+      </c>
+      <c r="R10" s="12">
+        <f t="shared" si="4"/>
+        <v>3.984163908796487E-2</v>
+      </c>
+      <c r="S10" s="12">
+        <v>3.8773892866059465E-2</v>
+      </c>
+      <c r="T10" s="3">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="H11" s="12"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="12">
+        <f t="shared" si="3"/>
+        <v>6.2195484254307778E-2</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0</v>
+      </c>
+      <c r="R11" s="12">
+        <f t="shared" si="4"/>
+        <v>0.16431335787465107</v>
+      </c>
+      <c r="S11" s="12">
+        <v>0.13668328904482138</v>
+      </c>
+      <c r="T11" s="3">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O12" s="10"/>
+      <c r="P12" s="12">
+        <f t="shared" si="3"/>
+        <v>9.7625703998253016E-2</v>
+      </c>
+      <c r="Q12" s="12">
+        <f>E41</f>
+        <v>0.64794685990338152</v>
+      </c>
+      <c r="R12" s="12">
+        <f t="shared" si="4"/>
+        <v>0.35283289635998394</v>
+      </c>
+      <c r="S12" s="12">
+        <v>0.33952593834448219</v>
+      </c>
+      <c r="T12" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="H13" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B14" s="15">
+      <c r="O13" s="11"/>
+      <c r="P13" s="12">
+        <f t="shared" si="3"/>
+        <v>3.3321906851318611E-2</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0</v>
+      </c>
+      <c r="R13" s="12">
+        <f t="shared" si="4"/>
+        <v>0.24715508454362833</v>
+      </c>
+      <c r="S13" s="12">
+        <v>0.19695300237092336</v>
+      </c>
+      <c r="T13" s="3">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="14">
         <v>1</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>0.5</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>6</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <v>5</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <v>3</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="14">
         <v>8</v>
       </c>
       <c r="H14" s="12">
         <f>H21</f>
         <v>0.27737594649359354</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B15" s="15">
+      <c r="S14" s="3">
+        <f>SUM(S8:S13)</f>
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B15" s="14">
         <f>1/C14</f>
         <v>2</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="14">
         <v>1</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>9</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>9</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <v>6</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="14">
         <v>9</v>
       </c>
       <c r="H15" s="12">
-        <f t="shared" ref="H15:H19" si="3">H22</f>
+        <f t="shared" ref="H15:H19" si="6">H22</f>
         <v>0.47514816338345756</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B16" s="15">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B16" s="14">
         <f>1/D14</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <f>1/D15</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="14">
         <v>1</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="14">
         <v>1</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <v>0.5</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="14">
         <v>2</v>
       </c>
       <c r="H16" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.4332795019069527E-2</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <f>1/E14</f>
         <v>0.2</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <f>1/E15</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="14">
         <f>1/E16</f>
         <v>1</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="14">
         <v>1</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="14">
         <v>0.5</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="14">
         <v>3</v>
       </c>
       <c r="H17" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.2195484254307778E-2</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <f>1/F14</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <f>1/F15</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <f>1/F16</f>
         <v>2</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="14">
         <f>1/F17</f>
         <v>2</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <v>1</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="14">
         <v>3</v>
       </c>
       <c r="H18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9.7625703998253016E-2</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <f>1/G14</f>
         <v>0.125</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <f>1/G15</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="14">
         <f>1/G16</f>
         <v>0.5</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="14">
         <f>1/G17</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="14">
         <f>1/G18</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="14">
         <v>1</v>
       </c>
       <c r="H19" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.3321906851318611E-2</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B20" s="3">
-        <f t="shared" ref="B20:G20" si="4">SUM(B14:B19)</f>
+        <f t="shared" ref="B20:G20" si="7">SUM(B14:B19)</f>
         <v>3.8250000000000002</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>19.5</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>18.333333333333332</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>11.333333333333334</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" ref="H20:H26" si="5">1/6*SUM(B20:G20)</f>
+        <f t="shared" ref="H20:H26" si="8">1/6*SUM(B20:G20)</f>
         <v>13.498611111111112</v>
       </c>
       <c r="I20" s="3" t="s">
@@ -3767,34 +4563,34 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B21" s="3">
-        <f t="shared" ref="B21:G21" si="6">B14/B20</f>
+        <f t="shared" ref="B21:G21" si="9">B14/B20</f>
         <v>0.26143790849673204</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.25</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.30769230769230771</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.27272727272727276</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.26470588235294118</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.30769230769230771</v>
       </c>
       <c r="H21" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.27737594649359354</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="12">
         <f t="array" ref="I21:I26">MMULT(B14:G19,H21:H26)</f>
         <v>1.7113765863765864</v>
       </c>
@@ -3805,186 +4601,186 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B22" s="3">
-        <f t="shared" ref="B22:G22" si="7">B15/B20</f>
+        <f t="shared" ref="B22:G22" si="10">B15/B20</f>
         <v>0.52287581699346408</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.46153846153846156</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.49090909090909096</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.52941176470588236</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.34615384615384615</v>
       </c>
       <c r="H22" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.47514816338345756</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="12">
         <v>2.964305955482426</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" ref="J22:J26" si="8">I22/H22</f>
+        <f t="shared" ref="J22:J26" si="11">I22/H22</f>
         <v>6.2386981239158237</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B23" s="3">
-        <f t="shared" ref="B23:G23" si="9">B16/B20</f>
+        <f t="shared" ref="B23:G23" si="12">B16/B20</f>
         <v>4.3572984749455333E-2</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>5.454545454545455E-2</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>4.4117647058823525E-2</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H23" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5.4332795019069527E-2</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="12">
         <v>0.33100850976667967</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>6.092241520991208</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B24" s="3">
-        <f t="shared" ref="B24:G24" si="10">B17/B20</f>
+        <f t="shared" ref="B24:G24" si="13">B17/B20</f>
         <v>5.2287581699346407E-2</v>
       </c>
       <c r="C24" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>5.454545454545455E-2</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4.4117647058823525E-2</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.11538461538461539</v>
       </c>
       <c r="H24" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6.2195484254307778E-2</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="12">
         <v>0.3735762815011181</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>6.0064856151553077</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B25" s="3">
-        <f t="shared" ref="B25:G25" si="11">B18/B20</f>
+        <f t="shared" ref="B25:G25" si="14">B18/B20</f>
         <v>8.7145969498910666E-2</v>
       </c>
       <c r="C25" s="3">
+        <f t="shared" si="14"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="14"/>
+        <v>0.10256410256410256</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="14"/>
+        <v>0.1090909090909091</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="14"/>
+        <v>8.8235294117647051E-2</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="14"/>
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="H25" s="12">
+        <f t="shared" si="8"/>
+        <v>9.7625703998253016E-2</v>
+      </c>
+      <c r="I25" s="12">
+        <v>0.60229799249407079</v>
+      </c>
+      <c r="J25" s="3">
         <f t="shared" si="11"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D25" s="3">
-        <f t="shared" si="11"/>
-        <v>0.10256410256410256</v>
-      </c>
-      <c r="E25" s="3">
-        <f t="shared" si="11"/>
-        <v>0.1090909090909091</v>
-      </c>
-      <c r="F25" s="3">
-        <f t="shared" si="11"/>
-        <v>8.8235294117647051E-2</v>
-      </c>
-      <c r="G25" s="3">
-        <f t="shared" si="11"/>
-        <v>0.11538461538461539</v>
-      </c>
-      <c r="H25" s="12">
-        <f t="shared" si="5"/>
-        <v>9.7625703998253016E-2</v>
-      </c>
-      <c r="I25" s="3">
-        <v>0.60229799249407079</v>
-      </c>
-      <c r="J25" s="3">
-        <f t="shared" si="8"/>
         <v>6.1694611954332101</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B26" s="3">
-        <f t="shared" ref="B26:G26" si="12">B19/B20</f>
+        <f t="shared" ref="B26:G26" si="15">B19/B20</f>
         <v>3.2679738562091505E-2</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1.8181818181818181E-2</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>2.9411764705882349E-2</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>3.8461538461538464E-2</v>
       </c>
       <c r="H26" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3.3321906851318611E-2</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="12">
         <v>0.20122826746601255</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>6.038918131662971</v>
       </c>
       <c r="K26" s="3" t="s">
@@ -3998,11 +4794,15 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="H27" s="3">
+        <f>SUM(H21:H26)</f>
+        <v>1</v>
+      </c>
       <c r="J27" s="3">
         <f>SUM(J21:J26)</f>
         <v>36.715685602476171</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="12">
         <f>J27/6</f>
         <v>6.1192809337460288</v>
       </c>
@@ -4037,7 +4837,7 @@
       </c>
       <c r="E33" s="12">
         <f>E39</f>
-        <v>8.5144927536231887E-2</v>
+        <v>0.12218196457326892</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.15">
@@ -4052,8 +4852,8 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E34" s="12">
-        <f t="shared" ref="E34:E35" si="13">E40</f>
-        <v>0.15579710144927533</v>
+        <f t="shared" ref="E34:E35" si="16">E40</f>
+        <v>0.2298711755233494</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.15">
@@ -4069,8 +4869,8 @@
         <v>1</v>
       </c>
       <c r="E35" s="12">
-        <f t="shared" si="13"/>
-        <v>0.42572463768115942</v>
+        <f t="shared" si="16"/>
+        <v>0.64794685990338152</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.15">
@@ -4093,11 +4893,11 @@
         <v>8</v>
       </c>
       <c r="C37" s="3">
-        <f t="shared" ref="C37:D37" si="14">C36</f>
+        <f t="shared" ref="C37:D37" si="17">C36</f>
         <v>4.5</v>
       </c>
       <c r="D37" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1.5333333333333332</v>
       </c>
     </row>
@@ -4107,11 +4907,11 @@
         <v>8</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" ref="C38:D38" si="15">C36</f>
+        <f t="shared" ref="C38:D38" si="18">C36</f>
         <v>4.5</v>
       </c>
       <c r="D38" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1.5333333333333332</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -4138,66 +4938,66 @@
         <v>0.13043478260869568</v>
       </c>
       <c r="E39" s="12">
-        <f>1/3*SUM(B39,D39)</f>
-        <v>8.5144927536231887E-2</v>
-      </c>
-      <c r="F39" s="3">
+        <f>1/3*SUM(B39:D39)</f>
+        <v>0.12218196457326892</v>
+      </c>
+      <c r="F39" s="12">
         <f t="array" ref="F39:F41">MMULT(B33:D35,E39:E41)</f>
-        <v>0.24818840579710144</v>
+        <v>0.36670692431561991</v>
       </c>
       <c r="G39" s="3">
         <f>F39/E39</f>
-        <v>2.9148936170212765</v>
+        <v>3.0013179571663917</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B40" s="3">
-        <f t="shared" ref="B40:D40" si="16">B34/B37</f>
+        <f t="shared" ref="B40:D40" si="19">B34/B37</f>
         <v>0.25</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D40" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.21739130434782608</v>
       </c>
       <c r="E40" s="12">
-        <f t="shared" ref="E40:E41" si="17">1/3*SUM(B40,D40)</f>
-        <v>0.15579710144927533</v>
-      </c>
-      <c r="F40" s="3">
-        <v>0.46799516908212557</v>
+        <f t="shared" ref="E40:E41" si="20">1/3*SUM(B40:D40)</f>
+        <v>0.2298711755233494</v>
+      </c>
+      <c r="F40" s="12">
+        <v>0.69021739130434778</v>
       </c>
       <c r="G40" s="3">
-        <f t="shared" ref="G40:G41" si="18">F40/E40</f>
-        <v>3.0038759689922485</v>
+        <f t="shared" ref="G40:G41" si="21">F40/E40</f>
+        <v>3.0026269702276709</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B41" s="3">
-        <f t="shared" ref="B41:D41" si="19">B35/B38</f>
+        <f t="shared" ref="B41:D41" si="22">B35/B38</f>
         <v>0.625</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D41" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0.65217391304347827</v>
       </c>
       <c r="E41" s="12">
-        <f t="shared" si="17"/>
-        <v>0.42572463768115942</v>
-      </c>
-      <c r="F41" s="3">
-        <v>1.3188405797101448</v>
+        <f t="shared" si="20"/>
+        <v>0.64794685990338152</v>
+      </c>
+      <c r="F41" s="12">
+        <v>1.9484702093397743</v>
       </c>
       <c r="G41" s="3">
-        <f t="shared" si="18"/>
-        <v>3.0978723404255315</v>
+        <f t="shared" si="21"/>
+        <v>3.0071450761105933</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>13</v>
@@ -4210,21 +5010,25 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="E42" s="3">
+        <f>SUM(E39:E41)</f>
+        <v>0.99999999999999978</v>
+      </c>
       <c r="G42" s="3">
         <f>SUM(G39:G41)</f>
-        <v>9.0166419264390569</v>
-      </c>
-      <c r="H42" s="3">
+        <v>9.0110900035046555</v>
+      </c>
+      <c r="H42" s="12">
         <f>G42/3</f>
-        <v>3.0055473088130191</v>
+        <v>3.0036966678348853</v>
       </c>
       <c r="I42" s="12">
         <f>(H42-3)/2</f>
-        <v>2.7736544065095625E-3</v>
-      </c>
-      <c r="J42" s="14">
+        <v>1.8483339174426572E-3</v>
+      </c>
+      <c r="J42" s="12">
         <f>I42/0.58</f>
-        <v>4.7821627698440734E-3</v>
+        <v>3.1867826162804438E-3</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.15">
@@ -4258,7 +5062,7 @@
       </c>
       <c r="H47" s="12">
         <f>H59</f>
-        <v>1.2499999999999999E-2</v>
+        <v>3.3405366386780107E-2</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.15">
@@ -4282,8 +5086,8 @@
         <v>0.5</v>
       </c>
       <c r="H48" s="12">
-        <f t="shared" ref="H48:H52" si="20">H60</f>
-        <v>6.25E-2</v>
+        <f t="shared" ref="H48:H52" si="23">H60</f>
+        <v>0.1624516557469915</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.15">
@@ -4308,8 +5112,8 @@
         <v>0.2</v>
       </c>
       <c r="H49" s="12">
-        <f t="shared" si="20"/>
-        <v>1.2499999999999999E-2</v>
+        <f t="shared" si="23"/>
+        <v>3.984163908796487E-2</v>
       </c>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.15">
@@ -4335,8 +5139,8 @@
         <v>0.5</v>
       </c>
       <c r="H50" s="12">
-        <f t="shared" si="20"/>
-        <v>7.4999999999999997E-2</v>
+        <f t="shared" si="23"/>
+        <v>0.16431335787465107</v>
       </c>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.15">
@@ -4363,8 +5167,8 @@
         <v>2</v>
       </c>
       <c r="H51" s="12">
-        <f t="shared" si="20"/>
-        <v>9.1666666666666674E-2</v>
+        <f t="shared" si="23"/>
+        <v>0.35283289635998394</v>
       </c>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.15">
@@ -4392,8 +5196,8 @@
         <v>1</v>
       </c>
       <c r="H52" s="12">
-        <f t="shared" si="20"/>
-        <v>7.9166666666666663E-2</v>
+        <f t="shared" si="23"/>
+        <v>0.24715508454362833</v>
       </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.15">
@@ -4402,23 +5206,23 @@
         <v>30</v>
       </c>
       <c r="C53" s="3">
-        <f t="shared" ref="C53:G53" si="21">SUM(C47:C52)</f>
+        <f t="shared" ref="C53:G53" si="24">SUM(C47:C52)</f>
         <v>6.4</v>
       </c>
       <c r="D53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>24</v>
       </c>
       <c r="E53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>7.3333333333333339</v>
       </c>
       <c r="F53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>2.6111111111111112</v>
       </c>
       <c r="G53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>4.3250000000000002</v>
       </c>
     </row>
@@ -4428,23 +5232,23 @@
         <v>30</v>
       </c>
       <c r="C54" s="3">
-        <f t="shared" ref="C54:G54" si="22">C53</f>
+        <f t="shared" ref="C54:G54" si="25">C53</f>
         <v>6.4</v>
       </c>
       <c r="D54" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>24</v>
       </c>
       <c r="E54" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>7.3333333333333339</v>
       </c>
       <c r="F54" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>2.6111111111111112</v>
       </c>
       <c r="G54" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>4.3250000000000002</v>
       </c>
     </row>
@@ -4454,23 +5258,23 @@
         <v>30</v>
       </c>
       <c r="C55" s="3">
-        <f t="shared" ref="C55:G55" si="23">C53</f>
+        <f t="shared" ref="C55:G55" si="26">C53</f>
         <v>6.4</v>
       </c>
       <c r="D55" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>24</v>
       </c>
       <c r="E55" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>7.3333333333333339</v>
       </c>
       <c r="F55" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>2.6111111111111112</v>
       </c>
       <c r="G55" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>4.3250000000000002</v>
       </c>
     </row>
@@ -4480,23 +5284,23 @@
         <v>30</v>
       </c>
       <c r="C56" s="3">
-        <f t="shared" ref="C56:G56" si="24">C53</f>
+        <f t="shared" ref="C56:G56" si="27">C53</f>
         <v>6.4</v>
       </c>
       <c r="D56" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>24</v>
       </c>
       <c r="E56" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>7.3333333333333339</v>
       </c>
       <c r="F56" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>2.6111111111111112</v>
       </c>
       <c r="G56" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>4.3250000000000002</v>
       </c>
     </row>
@@ -4506,23 +5310,23 @@
         <v>30</v>
       </c>
       <c r="C57" s="3">
-        <f t="shared" ref="C57:G57" si="25">C53</f>
+        <f t="shared" ref="C57:G57" si="28">C53</f>
         <v>6.4</v>
       </c>
       <c r="D57" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>24</v>
       </c>
       <c r="E57" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>7.3333333333333339</v>
       </c>
       <c r="F57" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>2.6111111111111112</v>
       </c>
       <c r="G57" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>4.3250000000000002</v>
       </c>
     </row>
@@ -4532,23 +5336,23 @@
         <v>30</v>
       </c>
       <c r="C58" s="3">
-        <f t="shared" ref="C58:G58" si="26">C53</f>
+        <f t="shared" ref="C58:G58" si="29">C53</f>
         <v>6.4</v>
       </c>
       <c r="D58" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>24</v>
       </c>
       <c r="E58" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>7.3333333333333339</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>2.6111111111111112</v>
       </c>
       <c r="G58" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>4.3250000000000002</v>
       </c>
       <c r="H58" s="3" t="s">
@@ -4567,221 +5371,221 @@
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="C59" s="3">
-        <f t="shared" ref="C59:G59" si="27">C47/C53</f>
+        <f t="shared" ref="C59:G59" si="30">C47/C53</f>
         <v>3.125E-2</v>
       </c>
       <c r="D59" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E59" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>2.2727272727272724E-2</v>
       </c>
       <c r="F59" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>4.2553191489361701E-2</v>
       </c>
       <c r="G59" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="H59" s="12">
-        <f>1/6*SUM(B59,D59)</f>
-        <v>1.2499999999999999E-2</v>
-      </c>
-      <c r="I59" s="3">
+        <f>1/6*SUM(B59:G59)</f>
+        <v>3.3405366386780107E-2</v>
+      </c>
+      <c r="I59" s="12">
         <f t="array" ref="I59:I64">MMULT(B47:G52,H59:H64)</f>
-        <v>7.0081018518518515E-2</v>
+        <v>0.20322093698898133</v>
       </c>
       <c r="J59" s="3">
         <f>I59/H59</f>
-        <v>5.6064814814814818</v>
+        <v>6.0834817566738115</v>
       </c>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B60" s="3">
-        <f t="shared" ref="B60:G60" si="28">B48/B54</f>
+        <f t="shared" ref="B60:G60" si="31">B48/B54</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="C60" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0.15625</v>
       </c>
       <c r="D60" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0.20833333333333334</v>
       </c>
       <c r="E60" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="F60" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0.19148936170212766</v>
       </c>
       <c r="G60" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0.11560693641618497</v>
       </c>
       <c r="H60" s="12">
-        <f t="shared" ref="H60:H64" si="29">1/6*SUM(B60,D60)</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="I60" s="3">
-        <v>0.34791666666666665</v>
+        <f t="shared" ref="H60:H64" si="32">1/6*SUM(B60:G60)</f>
+        <v>0.1624516557469915</v>
+      </c>
+      <c r="I60" s="12">
+        <v>0.99299403144717369</v>
       </c>
       <c r="J60" s="3">
-        <f t="shared" ref="J60:J64" si="30">I60/H60</f>
-        <v>5.5666666666666664</v>
+        <f t="shared" ref="J60:J64" si="33">I60/H60</f>
+        <v>6.1125510040581004</v>
       </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B61" s="3">
-        <f t="shared" ref="B61:G61" si="31">B49/B55</f>
+        <f t="shared" ref="B61:G61" si="34">B49/B55</f>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="C61" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>3.125E-2</v>
       </c>
       <c r="D61" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E61" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>2.2727272727272724E-2</v>
       </c>
       <c r="F61" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>6.3829787234042548E-2</v>
       </c>
       <c r="G61" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>4.6242774566473986E-2</v>
       </c>
       <c r="H61" s="12">
-        <f t="shared" si="29"/>
-        <v>1.2499999999999999E-2</v>
-      </c>
-      <c r="I61" s="3">
-        <v>8.1111111111111106E-2</v>
+        <f t="shared" si="32"/>
+        <v>3.984163908796487E-2</v>
+      </c>
+      <c r="I61" s="12">
+        <v>0.24135939590530811</v>
       </c>
       <c r="J61" s="3">
-        <f t="shared" si="30"/>
-        <v>6.4888888888888889</v>
+        <f t="shared" si="33"/>
+        <v>6.0579685331825752</v>
       </c>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B62" s="3">
-        <f t="shared" ref="B62:G62" si="32">B50/B56</f>
+        <f t="shared" ref="B62:G62" si="35">B50/B56</f>
         <v>0.2</v>
       </c>
       <c r="C62" s="3">
+        <f t="shared" si="35"/>
+        <v>0.15625</v>
+      </c>
+      <c r="D62" s="3">
+        <f t="shared" si="35"/>
+        <v>0.25</v>
+      </c>
+      <c r="E62" s="3">
+        <f t="shared" si="35"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="F62" s="3">
+        <f t="shared" si="35"/>
+        <v>0.1276595744680851</v>
+      </c>
+      <c r="G62" s="3">
+        <f t="shared" si="35"/>
+        <v>0.11560693641618497</v>
+      </c>
+      <c r="H62" s="12">
         <f t="shared" si="32"/>
-        <v>0.15625</v>
-      </c>
-      <c r="D62" s="3">
-        <f t="shared" si="32"/>
-        <v>0.25</v>
-      </c>
-      <c r="E62" s="3">
-        <f t="shared" si="32"/>
-        <v>0.13636363636363635</v>
-      </c>
-      <c r="F62" s="3">
-        <f t="shared" si="32"/>
-        <v>0.1276595744680851</v>
-      </c>
-      <c r="G62" s="3">
-        <f t="shared" si="32"/>
-        <v>0.11560693641618497</v>
-      </c>
-      <c r="H62" s="12">
-        <f t="shared" si="29"/>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="I62" s="3">
-        <v>0.35763888888888895</v>
+        <v>0.16431335787465107</v>
+      </c>
+      <c r="I62" s="12">
+        <v>1.0074355541952547</v>
       </c>
       <c r="J62" s="3">
-        <f t="shared" si="30"/>
-        <v>4.7685185185185199</v>
+        <f t="shared" si="33"/>
+        <v>6.1311847510522677</v>
       </c>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B63" s="3">
-        <f t="shared" ref="B63:G63" si="33">B51/B57</f>
+        <f t="shared" ref="B63:G63" si="36">B51/B57</f>
         <v>0.3</v>
       </c>
       <c r="C63" s="3">
+        <f t="shared" si="36"/>
+        <v>0.3125</v>
+      </c>
+      <c r="D63" s="3">
+        <f t="shared" si="36"/>
+        <v>0.25</v>
+      </c>
+      <c r="E63" s="3">
+        <f t="shared" si="36"/>
+        <v>0.40909090909090906</v>
+      </c>
+      <c r="F63" s="3">
+        <f t="shared" si="36"/>
+        <v>0.38297872340425532</v>
+      </c>
+      <c r="G63" s="3">
+        <f t="shared" si="36"/>
+        <v>0.46242774566473988</v>
+      </c>
+      <c r="H63" s="12">
+        <f t="shared" si="32"/>
+        <v>0.35283289635998394</v>
+      </c>
+      <c r="I63" s="12">
+        <v>2.2046845825739867</v>
+      </c>
+      <c r="J63" s="3">
         <f t="shared" si="33"/>
-        <v>0.3125</v>
-      </c>
-      <c r="D63" s="3">
-        <f t="shared" si="33"/>
-        <v>0.25</v>
-      </c>
-      <c r="E63" s="3">
-        <f t="shared" si="33"/>
-        <v>0.40909090909090906</v>
-      </c>
-      <c r="F63" s="3">
-        <f t="shared" si="33"/>
-        <v>0.38297872340425532</v>
-      </c>
-      <c r="G63" s="3">
-        <f t="shared" si="33"/>
-        <v>0.46242774566473988</v>
-      </c>
-      <c r="H63" s="12">
-        <f t="shared" si="29"/>
-        <v>9.1666666666666674E-2</v>
-      </c>
-      <c r="I63" s="3">
-        <v>0.78749999999999998</v>
-      </c>
-      <c r="J63" s="3">
-        <f t="shared" si="30"/>
-        <v>8.5909090909090899</v>
+        <v>6.2485233245502672</v>
       </c>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B64" s="3">
-        <f t="shared" ref="B64:G64" si="34">B52/B58</f>
+        <f t="shared" ref="B64:G64" si="37">B52/B58</f>
         <v>0.26666666666666666</v>
       </c>
       <c r="C64" s="3">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0.3125</v>
       </c>
       <c r="D64" s="3">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0.20833333333333334</v>
       </c>
       <c r="E64" s="3">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0.19148936170212766</v>
       </c>
       <c r="G64" s="3">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0.23121387283236994</v>
       </c>
       <c r="H64" s="12">
-        <f t="shared" si="29"/>
-        <v>7.9166666666666663E-2</v>
-      </c>
-      <c r="I64" s="3">
-        <v>0.5625</v>
+        <f t="shared" si="32"/>
+        <v>0.24715508454362833</v>
+      </c>
+      <c r="I64" s="12">
+        <v>1.5435526865009705</v>
       </c>
       <c r="J64" s="3">
-        <f t="shared" si="30"/>
-        <v>7.1052631578947372</v>
+        <f t="shared" si="33"/>
+        <v>6.2452799194932176</v>
       </c>
       <c r="K64" s="3" t="s">
         <v>13</v>
@@ -4793,22 +5597,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="10:13" x14ac:dyDescent="0.15">
+    <row r="65" spans="8:13" x14ac:dyDescent="0.15">
+      <c r="H65" s="3">
+        <f>SUM(H59:H64)</f>
+        <v>0.99999999999999978</v>
+      </c>
       <c r="J65" s="3">
         <f>SUM(J59:J64)</f>
-        <v>38.126727804359383</v>
-      </c>
-      <c r="K65" s="3">
+        <v>36.878989289010235</v>
+      </c>
+      <c r="K65" s="12">
         <f>J65/6</f>
-        <v>6.3544546340598975</v>
+        <v>6.1464982148350389</v>
       </c>
       <c r="L65" s="12">
         <f>(K65-6)/5</f>
-        <v>7.0890926811979504E-2</v>
+        <v>2.9299642967007777E-2</v>
       </c>
       <c r="M65" s="12">
         <f>L65/1.24</f>
-        <v>5.7170102267725405E-2</v>
+        <v>2.3628744328232077E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4870,7 +5678,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A3" s="17">
+      <c r="A3" s="16">
         <v>0.16666666666666666</v>
       </c>
       <c r="B3" s="13">
@@ -4953,7 +5761,7 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="17">
         <v>41276</v>
       </c>
       <c r="J11">
@@ -4990,10 +5798,10 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="H13" s="18">
+      <c r="H13" s="17">
         <v>41280</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="17">
         <v>41283</v>
       </c>
       <c r="J13">
@@ -5002,7 +5810,7 @@
       <c r="K13">
         <v>1</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="17">
         <v>41276</v>
       </c>
       <c r="M13">
@@ -5010,10 +5818,10 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="H14" s="18">
+      <c r="H14" s="17">
         <v>41279</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="17">
         <v>41283</v>
       </c>
       <c r="J14">
@@ -5022,7 +5830,7 @@
       <c r="K14">
         <v>1</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="17">
         <v>41276</v>
       </c>
       <c r="M14">
@@ -5030,10 +5838,10 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="H15" s="18">
+      <c r="H15" s="17">
         <v>41277</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="17">
         <v>41280</v>
       </c>
       <c r="J15">
@@ -5050,19 +5858,19 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="H16" s="18">
+      <c r="H16" s="17">
         <v>41282</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="17">
         <v>41283</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="17">
         <v>41276</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="17">
         <v>41277</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L16" s="17">
         <v>41277</v>
       </c>
       <c r="M16">
@@ -5110,7 +5918,7 @@
       </c>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.15">
-      <c r="E21" s="17">
+      <c r="E21" s="16">
         <v>0.16666666666666666</v>
       </c>
       <c r="F21" s="13">

</xml_diff>

<commit_message>
accomplish the part of AHP.
</commit_message>
<xml_diff>
--- a/判断矩阵权重计算.xlsx
+++ b/判断矩阵权重计算.xlsx
@@ -15,14 +15,14 @@
     <definedName name="_Ref375656298" localSheetId="0">Sheet1!$A$1</definedName>
     <definedName name="_Ref375658416" localSheetId="0">Sheet1!$A$11</definedName>
     <definedName name="_Ref375658423" localSheetId="0">Sheet1!$A$31</definedName>
-    <definedName name="_Ref375658432" localSheetId="0">Sheet1!$A$44</definedName>
+    <definedName name="_Ref375658432" localSheetId="0">Sheet1!$B$44</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>W</t>
   </si>
@@ -30,125 +30,40 @@
     <t>权重</t>
   </si>
   <si>
-    <r>
-      <t>表</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 1.7 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>判断矩阵</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>W-A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>及相关权重</t>
-    </r>
-  </si>
-  <si>
-    <t>及相关权重</t>
-  </si>
-  <si>
-    <t>表 1.8 判断矩阵</t>
-  </si>
-  <si>
-    <r>
-      <t>表</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 1.9 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>判断矩阵</t>
-    </r>
-  </si>
-  <si>
-    <t>表 1.10 判断矩阵</t>
-  </si>
-  <si>
     <t>Aw</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>3lemda</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>lemda</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>ci</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>cr</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>6lemda</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>lemda</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>RI总</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>CI总</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>cr总</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>组合权重及总排序</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>因素</t>
@@ -159,6 +74,59 @@
   <si>
     <t>总排序</t>
   </si>
+  <si>
+    <t>A1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>B1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>B2</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>表 1.8 判断矩阵及相关权重</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>表 1.9 判断矩阵及相关权重</t>
+  </si>
+  <si>
+    <t>表 1.10 判断矩阵及相关权重</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>表 1.7 判断矩阵W-A及相关权重</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1.11 各因素组合权重及总排序</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>CR总</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -167,7 +135,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,22 +159,9 @@
     <font>
       <sz val="10.5"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -222,6 +177,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,7 +195,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -239,62 +203,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="12" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -303,19 +220,42 @@
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="12" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="12" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="12" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -724,16 +664,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -767,8 +707,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1114425" y="1895475"/>
-          <a:ext cx="390525" cy="257175"/>
+          <a:off x="2828925" y="2124075"/>
+          <a:ext cx="390525" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2089,16 +2029,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2132,7 +2072,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1028700" y="4876800"/>
+          <a:off x="2819400" y="5257800"/>
           <a:ext cx="390525" cy="257175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2154,16 +2094,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2197,7 +2137,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1571625" y="8039100"/>
+          <a:off x="2819400" y="7667625"/>
           <a:ext cx="390525" cy="257175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3062,591 +3002,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="54" name="图片 53"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="11591925" y="1200150"/>
-          <a:ext cx="161925" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="55" name="图片 54"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="12277725" y="1200150"/>
-          <a:ext cx="161925" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="56" name="图片 55"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="12963525" y="1200150"/>
-          <a:ext cx="161925" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="57" name="图片 56"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10906125" y="1419225"/>
-          <a:ext cx="161925" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="58" name="图片 57"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10906125" y="1638300"/>
-          <a:ext cx="161925" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="59" name="图片 58"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10906125" y="1838325"/>
-          <a:ext cx="161925" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="60" name="图片 59"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10906125" y="2038350"/>
-          <a:ext cx="152400" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="68" name="图片 67"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10906125" y="2238375"/>
-          <a:ext cx="161925" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="70" name="图片 69"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10906125" y="2438400"/>
-          <a:ext cx="161925" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -3986,75 +3341,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T65"/>
+  <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L56" sqref="L56"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="9" style="3"/>
-    <col min="4" max="4" width="11.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9" style="3"/>
-    <col min="8" max="8" width="17.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9" style="3"/>
-    <col min="10" max="10" width="11.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="3"/>
+    <col min="1" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="1"/>
+    <col min="8" max="8" width="17.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="1"/>
+    <col min="10" max="10" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9" style="1"/>
+    <col min="15" max="15" width="10.75" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.75" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.25" style="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9.875" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="2"/>
+      <c r="B1" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
-      <c r="L1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="12">
-        <f>E6*1.24+E7*0.58+E8*1.24</f>
-        <v>1.1878695652173912</v>
-      </c>
-      <c r="M2" s="12">
-        <f>L27*E6+I42*E7+L65*E8</f>
-        <v>2.6350369765900963E-2</v>
-      </c>
-      <c r="N2" s="12">
-        <f>M2/L2</f>
-        <v>2.2182881469042941E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="9"/>
-      <c r="B3" s="1">
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A3" s="11"/>
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="5">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>0.16666666666666666</v>
       </c>
       <c r="E3" s="12">
@@ -4062,16 +3403,16 @@
         <v>0.14347826086956519</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <f>1/C3</f>
         <v>0.5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <v>0.1111111111111111</v>
       </c>
       <c r="E4" s="12">
@@ -4079,1548 +3420,1598 @@
         <v>7.898550724637679E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="15">
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A5" s="10"/>
+      <c r="B5" s="5">
         <f>1/D3</f>
         <v>6</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="5">
         <f>1/D4</f>
         <v>9</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="0"/>
         <v>0.77753623188405785</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="12">
+      <c r="F5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B6" s="3">
         <f>B3/(B3+B4+B5)</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="3">
         <f>C3/(C3+C4+C5)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="3">
         <f>D3/(D3+D4+D5)</f>
         <v>0.13043478260869565</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="3">
         <f>1/3*(B6+C6+D6)</f>
         <v>0.14347826086956519</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="3">
         <f t="array" ref="F6:F8">MMULT(B3:D5,E6:E8)</f>
         <v>0.43103864734299513</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="1">
         <f>F6/E6</f>
         <v>3.0042087542087543</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="12">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B7" s="3">
         <f>B4/(B4+B5+B3)</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="3">
         <f>C4/(C4+C5+C3)</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="3">
         <f>D4/(D4+D5+D3)</f>
         <v>8.6956521739130418E-2</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="3">
         <f t="shared" ref="E7:E8" si="1">1/3*(B7+C7+D7)</f>
         <v>7.898550724637679E-2</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="3">
         <v>0.23711755233494358</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="1">
         <f t="shared" ref="G7:G8" si="2">F7/E7</f>
         <v>3.0020387359836902</v>
       </c>
-      <c r="O7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="12">
+    </row>
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="3">
         <f>B5/(B5+B4+B3)</f>
         <v>0.8</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="3">
         <f>C5/(C5+C4+C3)</f>
         <v>0.75</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="3">
         <f>D5/(D5+D4+D3)</f>
         <v>0.78260869565217384</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="3">
         <f t="shared" si="1"/>
         <v>0.77753623188405785</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="3">
         <v>2.3492753623188403</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="1">
         <f t="shared" si="2"/>
         <v>3.02143522833178</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O8" s="18"/>
-      <c r="P8" s="12">
+      <c r="H8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="E9" s="1">
+        <f>SUM(E6:E8)</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="G9" s="1">
+        <f>SUM(G6:G8)</f>
+        <v>9.0276827185242254</v>
+      </c>
+      <c r="H9" s="3">
+        <f>G9/3</f>
+        <v>3.0092275728414086</v>
+      </c>
+      <c r="I9" s="3">
+        <f>(H9-3)/2</f>
+        <v>4.6137864207043133E-3</v>
+      </c>
+      <c r="J9" s="3">
+        <f>I9/0.58</f>
+        <v>7.9548041736281268E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B12" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="5">
+        <v>6</v>
+      </c>
+      <c r="E14" s="5">
+        <v>5</v>
+      </c>
+      <c r="F14" s="5">
+        <v>3</v>
+      </c>
+      <c r="G14" s="5">
+        <v>8</v>
+      </c>
+      <c r="H14" s="3">
         <f>H21</f>
         <v>0.27737594649359354</v>
       </c>
-      <c r="Q8" s="12">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B15" s="5">
+        <f>1/C14</f>
+        <v>2</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5">
+        <v>9</v>
+      </c>
+      <c r="E15" s="5">
+        <v>9</v>
+      </c>
+      <c r="F15" s="5">
+        <v>6</v>
+      </c>
+      <c r="G15" s="5">
+        <v>9</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" ref="H15:H19" si="3">H22</f>
+        <v>0.47514816338345756</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B16" s="5">
+        <f>1/D14</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C16" s="5">
+        <f>1/D15</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="5">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="3"/>
+        <v>5.4332795019069527E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B17" s="5">
+        <f>1/E14</f>
+        <v>0.2</v>
+      </c>
+      <c r="C17" s="5">
+        <f>1/E15</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D17" s="5">
+        <f>1/E16</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3">
+        <f t="shared" si="3"/>
+        <v>6.2195484254307778E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B18" s="5">
+        <f>1/F14</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C18" s="5">
+        <f>1/F15</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D18" s="5">
+        <f>1/F16</f>
+        <v>2</v>
+      </c>
+      <c r="E18" s="5">
+        <f>1/F17</f>
+        <v>2</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" si="3"/>
+        <v>9.7625703998253016E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B19" s="5">
+        <f>1/G14</f>
+        <v>0.125</v>
+      </c>
+      <c r="C19" s="5">
+        <f>1/G15</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D19" s="5">
+        <f>1/G16</f>
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="5">
+        <f>1/G17</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F19" s="5">
+        <f>1/G18</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="3"/>
+        <v>3.3321906851318611E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B20" s="1">
+        <f t="shared" ref="B20:G20" si="4">SUM(B14:B19)</f>
+        <v>3.8250000000000002</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="4"/>
+        <v>19.5</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="4"/>
+        <v>18.333333333333332</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="4"/>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" ref="H20:H26" si="5">1/6*SUM(B20:G20)</f>
+        <v>13.498611111111112</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B21" s="1">
+        <f t="shared" ref="B21:G21" si="6">B14/B20</f>
+        <v>0.26143790849673204</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="6"/>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="6"/>
+        <v>0.27272727272727276</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="6"/>
+        <v>0.26470588235294118</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="6"/>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" si="5"/>
+        <v>0.27737594649359354</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="array" ref="I21:I26">MMULT(B14:G19,H21:H26)</f>
+        <v>1.7113765863765864</v>
+      </c>
+      <c r="J21" s="1">
+        <f>I21/H21</f>
+        <v>6.1698810153176478</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B22" s="1">
+        <f t="shared" ref="B22:G22" si="7">B15/B20</f>
+        <v>0.52287581699346408</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="7"/>
+        <v>0.46153846153846156</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="7"/>
+        <v>0.49090909090909096</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="7"/>
+        <v>0.52941176470588236</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="7"/>
+        <v>0.34615384615384615</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" si="5"/>
+        <v>0.47514816338345756</v>
+      </c>
+      <c r="I22" s="3">
+        <v>2.964305955482426</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" ref="J22:J26" si="8">I22/H22</f>
+        <v>6.2386981239158237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B23" s="1">
+        <f t="shared" ref="B23:G23" si="9">B16/B20</f>
+        <v>4.3572984749455333E-2</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="9"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="9"/>
+        <v>5.128205128205128E-2</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="9"/>
+        <v>5.454545454545455E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="9"/>
+        <v>4.4117647058823525E-2</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="9"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" si="5"/>
+        <v>5.4332795019069527E-2</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.33100850976667967</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="8"/>
+        <v>6.092241520991208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B24" s="1">
+        <f t="shared" ref="B24:G24" si="10">B17/B20</f>
+        <v>5.2287581699346407E-2</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="10"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="10"/>
+        <v>5.128205128205128E-2</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="10"/>
+        <v>5.454545454545455E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="10"/>
+        <v>4.4117647058823525E-2</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="10"/>
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="5"/>
+        <v>6.2195484254307778E-2</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.3735762815011181</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="8"/>
+        <v>6.0064856151553077</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B25" s="1">
+        <f t="shared" ref="B25:G25" si="11">B18/B20</f>
+        <v>8.7145969498910666E-2</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="11"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="11"/>
+        <v>0.10256410256410256</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="11"/>
+        <v>0.1090909090909091</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="11"/>
+        <v>8.8235294117647051E-2</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="11"/>
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="H25" s="3">
+        <f t="shared" si="5"/>
+        <v>9.7625703998253016E-2</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.60229799249407079</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="8"/>
+        <v>6.1694611954332101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B26" s="1">
+        <f t="shared" ref="B26:G26" si="12">B19/B20</f>
+        <v>3.2679738562091505E-2</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="12"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="12"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="12"/>
+        <v>1.8181818181818181E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="12"/>
+        <v>2.9411764705882349E-2</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="12"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="H26" s="3">
+        <f t="shared" si="5"/>
+        <v>3.3321906851318611E-2</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.20122826746601255</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="8"/>
+        <v>6.038918131662971</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="H27" s="1">
+        <f>SUM(H21:H26)</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <f>SUM(J21:J26)</f>
+        <v>36.715685602476171</v>
+      </c>
+      <c r="K27" s="3">
+        <f>J27/6</f>
+        <v>6.1192809337460288</v>
+      </c>
+      <c r="L27" s="3">
+        <f>(K27-6)/5</f>
+        <v>2.3856186749205754E-2</v>
+      </c>
+      <c r="M27" s="3">
+        <f>L27/1.24</f>
+        <v>1.9238860281617545E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A30" s="2"/>
+      <c r="B30" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E33" s="3">
         <f>E39</f>
         <v>0.12218196457326892</v>
       </c>
-      <c r="R8" s="12">
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B34" s="1">
+        <f>1/C33</f>
+        <v>2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" ref="E34:E35" si="13">E40</f>
+        <v>0.2298711755233494</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B35" s="1">
+        <f>1/D33</f>
+        <v>5</v>
+      </c>
+      <c r="C35" s="1">
+        <f>1/D34</f>
+        <v>3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="13"/>
+        <v>0.64794685990338152</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B36" s="1">
+        <f>SUM(B33:B35)</f>
+        <v>8</v>
+      </c>
+      <c r="C36" s="1">
+        <f>SUM(C33:C35)</f>
+        <v>4.5</v>
+      </c>
+      <c r="D36" s="1">
+        <f>SUM(D33:D35)</f>
+        <v>1.5333333333333332</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B37" s="1">
+        <f>B36</f>
+        <v>8</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" ref="C37:D37" si="14">C36</f>
+        <v>4.5</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="14"/>
+        <v>1.5333333333333332</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B38" s="1">
+        <f>B36</f>
+        <v>8</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" ref="C38:D38" si="15">C36</f>
+        <v>4.5</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="15"/>
+        <v>1.5333333333333332</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B39" s="1">
+        <f>B33/B36</f>
+        <v>0.125</v>
+      </c>
+      <c r="C39" s="1">
+        <f>C33/C36</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D39" s="1">
+        <f>D33/D36</f>
+        <v>0.13043478260869568</v>
+      </c>
+      <c r="E39" s="3">
+        <f>1/3*SUM(B39:D39)</f>
+        <v>0.12218196457326892</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="array" ref="F39:F41">MMULT(B33:D35,E39:E41)</f>
+        <v>0.36670692431561991</v>
+      </c>
+      <c r="G39" s="1">
+        <f>F39/E39</f>
+        <v>3.0013179571663917</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B40" s="1">
+        <f t="shared" ref="B40:D40" si="16">B34/B37</f>
+        <v>0.25</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="16"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="16"/>
+        <v>0.21739130434782608</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" ref="E40:E41" si="17">1/3*SUM(B40:D40)</f>
+        <v>0.2298711755233494</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.69021739130434778</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" ref="G40:G41" si="18">F40/E40</f>
+        <v>3.0026269702276709</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B41" s="1">
+        <f t="shared" ref="B41:D41" si="19">B35/B38</f>
+        <v>0.625</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="19"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="19"/>
+        <v>0.65217391304347827</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="17"/>
+        <v>0.64794685990338152</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1.9484702093397743</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="18"/>
+        <v>3.0071450761105933</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="E42" s="1">
+        <f>SUM(E39:E41)</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="G42" s="1">
+        <f>SUM(G39:G41)</f>
+        <v>9.0110900035046555</v>
+      </c>
+      <c r="H42" s="3">
+        <f>G42/3</f>
+        <v>3.0036966678348853</v>
+      </c>
+      <c r="I42" s="3">
+        <f>(H42-3)/2</f>
+        <v>1.8483339174426572E-3</v>
+      </c>
+      <c r="J42" s="3">
+        <f>I42/0.58</f>
+        <v>3.1867826162804438E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B44" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="H47" s="3">
         <f>H59</f>
         <v>3.3405366386780107E-2</v>
       </c>
-      <c r="S8" s="12">
-        <f t="array" ref="S8:S13">MMULT(P8:R13,E6:E8)</f>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B48" s="1">
+        <f>1/C47</f>
+        <v>5</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
+        <v>5</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H48" s="3">
+        <f t="shared" ref="H48:H52" si="20">H60</f>
+        <v>0.1624516557469915</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B49" s="1">
+        <f>1/D47</f>
+        <v>1</v>
+      </c>
+      <c r="C49" s="1">
+        <f>1/D48</f>
+        <v>0.2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H49" s="3">
+        <f t="shared" si="20"/>
+        <v>3.984163908796487E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B50" s="1">
+        <f>1/E47</f>
+        <v>6</v>
+      </c>
+      <c r="C50" s="1">
+        <f>1/E48</f>
+        <v>1</v>
+      </c>
+      <c r="D50" s="1">
+        <f>1/E49</f>
+        <v>6</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H50" s="3">
+        <f t="shared" si="20"/>
+        <v>0.16431335787465107</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B51" s="1">
+        <f>1/F47</f>
+        <v>9</v>
+      </c>
+      <c r="C51" s="1">
+        <f>1/F48</f>
+        <v>2</v>
+      </c>
+      <c r="D51" s="1">
+        <f>1/F49</f>
+        <v>6</v>
+      </c>
+      <c r="E51" s="1">
+        <f>1/F50</f>
+        <v>3</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1">
+        <v>2</v>
+      </c>
+      <c r="H51" s="3">
+        <f t="shared" si="20"/>
+        <v>0.35283289635998394</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B52" s="1">
+        <f>1/G47</f>
+        <v>8</v>
+      </c>
+      <c r="C52" s="1">
+        <f>1/G48</f>
+        <v>2</v>
+      </c>
+      <c r="D52" s="1">
+        <f>1/G49</f>
+        <v>5</v>
+      </c>
+      <c r="E52" s="1">
+        <f>1/G50</f>
+        <v>2</v>
+      </c>
+      <c r="F52" s="1">
+        <f>1/G51</f>
+        <v>0.5</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1</v>
+      </c>
+      <c r="H52" s="3">
+        <f t="shared" si="20"/>
+        <v>0.24715508454362833</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B53" s="1">
+        <f>SUM(B47:B52)</f>
+        <v>30</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" ref="C53:G53" si="21">SUM(C47:C52)</f>
+        <v>6.4</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="21"/>
+        <v>24</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="21"/>
+        <v>7.3333333333333339</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="21"/>
+        <v>2.6111111111111112</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="21"/>
+        <v>4.3250000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B54" s="1">
+        <f>B53</f>
+        <v>30</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" ref="C54:G54" si="22">C53</f>
+        <v>6.4</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="22"/>
+        <v>24</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="22"/>
+        <v>7.3333333333333339</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="22"/>
+        <v>2.6111111111111112</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="22"/>
+        <v>4.3250000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B55" s="1">
+        <f>B53</f>
+        <v>30</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" ref="C55:G55" si="23">C53</f>
+        <v>6.4</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="23"/>
+        <v>24</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="23"/>
+        <v>7.3333333333333339</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="23"/>
+        <v>2.6111111111111112</v>
+      </c>
+      <c r="G55" s="1">
+        <f t="shared" si="23"/>
+        <v>4.3250000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B56" s="1">
+        <f>B53</f>
+        <v>30</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" ref="C56:G56" si="24">C53</f>
+        <v>6.4</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="24"/>
+        <v>24</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="24"/>
+        <v>7.3333333333333339</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="24"/>
+        <v>2.6111111111111112</v>
+      </c>
+      <c r="G56" s="1">
+        <f t="shared" si="24"/>
+        <v>4.3250000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B57" s="1">
+        <f>B53</f>
+        <v>30</v>
+      </c>
+      <c r="C57" s="1">
+        <f t="shared" ref="C57:G57" si="25">C53</f>
+        <v>6.4</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="25"/>
+        <v>24</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="25"/>
+        <v>7.3333333333333339</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="25"/>
+        <v>2.6111111111111112</v>
+      </c>
+      <c r="G57" s="1">
+        <f t="shared" si="25"/>
+        <v>4.3250000000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B58" s="1">
+        <f>B53</f>
+        <v>30</v>
+      </c>
+      <c r="C58" s="1">
+        <f t="shared" ref="C58:G58" si="26">C53</f>
+        <v>6.4</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" si="26"/>
+        <v>24</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="26"/>
+        <v>7.3333333333333339</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="26"/>
+        <v>2.6111111111111112</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="26"/>
+        <v>4.3250000000000002</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B59" s="1">
+        <f>B47/B53</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="C59" s="1">
+        <f t="shared" ref="C59:G59" si="27">C47/C53</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D59" s="1">
+        <f t="shared" si="27"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="27"/>
+        <v>2.2727272727272724E-2</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="27"/>
+        <v>4.2553191489361701E-2</v>
+      </c>
+      <c r="G59" s="1">
+        <f t="shared" si="27"/>
+        <v>2.8901734104046242E-2</v>
+      </c>
+      <c r="H59" s="3">
+        <f>1/6*SUM(B59:G59)</f>
+        <v>3.3405366386780107E-2</v>
+      </c>
+      <c r="I59" s="3">
+        <f t="array" ref="I59:I64">MMULT(B47:G52,H59:H64)</f>
+        <v>0.20322093698898133</v>
+      </c>
+      <c r="J59" s="1">
+        <f>I59/H59</f>
+        <v>6.0834817566738115</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B60" s="1">
+        <f t="shared" ref="B60:G60" si="28">B48/B54</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C60" s="1">
+        <f t="shared" si="28"/>
+        <v>0.15625</v>
+      </c>
+      <c r="D60" s="1">
+        <f t="shared" si="28"/>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" si="28"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="28"/>
+        <v>0.19148936170212766</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="28"/>
+        <v>0.11560693641618497</v>
+      </c>
+      <c r="H60" s="3">
+        <f t="shared" ref="H60:H64" si="29">1/6*SUM(B60:G60)</f>
+        <v>0.1624516557469915</v>
+      </c>
+      <c r="I60" s="3">
+        <v>0.99299403144717369</v>
+      </c>
+      <c r="J60" s="1">
+        <f t="shared" ref="J60:J64" si="30">I60/H60</f>
+        <v>6.1125510040581004</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B61" s="1">
+        <f t="shared" ref="B61:G61" si="31">B49/B55</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="C61" s="1">
+        <f t="shared" si="31"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D61" s="1">
+        <f t="shared" si="31"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="31"/>
+        <v>2.2727272727272724E-2</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="31"/>
+        <v>6.3829787234042548E-2</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" si="31"/>
+        <v>4.6242774566473986E-2</v>
+      </c>
+      <c r="H61" s="3">
+        <f t="shared" si="29"/>
+        <v>3.984163908796487E-2</v>
+      </c>
+      <c r="I61" s="3">
+        <v>0.24135939590530811</v>
+      </c>
+      <c r="J61" s="1">
+        <f t="shared" si="30"/>
+        <v>6.0579685331825752</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B62" s="1">
+        <f t="shared" ref="B62:G62" si="32">B50/B56</f>
+        <v>0.2</v>
+      </c>
+      <c r="C62" s="1">
+        <f t="shared" si="32"/>
+        <v>0.15625</v>
+      </c>
+      <c r="D62" s="1">
+        <f t="shared" si="32"/>
+        <v>0.25</v>
+      </c>
+      <c r="E62" s="1">
+        <f t="shared" si="32"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="32"/>
+        <v>0.1276595744680851</v>
+      </c>
+      <c r="G62" s="1">
+        <f t="shared" si="32"/>
+        <v>0.11560693641618497</v>
+      </c>
+      <c r="H62" s="3">
+        <f t="shared" si="29"/>
+        <v>0.16431335787465107</v>
+      </c>
+      <c r="I62" s="3">
+        <v>1.0074355541952547</v>
+      </c>
+      <c r="J62" s="1">
+        <f t="shared" si="30"/>
+        <v>6.1311847510522677</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B63" s="1">
+        <f t="shared" ref="B63:G63" si="33">B51/B57</f>
+        <v>0.3</v>
+      </c>
+      <c r="C63" s="1">
+        <f t="shared" si="33"/>
+        <v>0.3125</v>
+      </c>
+      <c r="D63" s="1">
+        <f t="shared" si="33"/>
+        <v>0.25</v>
+      </c>
+      <c r="E63" s="1">
+        <f t="shared" si="33"/>
+        <v>0.40909090909090906</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="33"/>
+        <v>0.38297872340425532</v>
+      </c>
+      <c r="G63" s="1">
+        <f t="shared" si="33"/>
+        <v>0.46242774566473988</v>
+      </c>
+      <c r="H63" s="3">
+        <f t="shared" si="29"/>
+        <v>0.35283289635998394</v>
+      </c>
+      <c r="I63" s="3">
+        <v>2.2046845825739867</v>
+      </c>
+      <c r="J63" s="1">
+        <f t="shared" si="30"/>
+        <v>6.2485233245502672</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B64" s="1">
+        <f t="shared" ref="B64:G64" si="34">B52/B58</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="C64" s="1">
+        <f t="shared" si="34"/>
+        <v>0.3125</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="34"/>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E64" s="1">
+        <f t="shared" si="34"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" si="34"/>
+        <v>0.19148936170212766</v>
+      </c>
+      <c r="G64" s="1">
+        <f t="shared" si="34"/>
+        <v>0.23121387283236994</v>
+      </c>
+      <c r="H64" s="3">
+        <f t="shared" si="29"/>
+        <v>0.24715508454362833</v>
+      </c>
+      <c r="I64" s="3">
+        <v>1.5435526865009705</v>
+      </c>
+      <c r="J64" s="1">
+        <f t="shared" si="30"/>
+        <v>6.2452799194932176</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="H65" s="1">
+        <f>SUM(H59:H64)</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="J65" s="1">
+        <f>SUM(J59:J64)</f>
+        <v>36.878989289010235</v>
+      </c>
+      <c r="K65" s="3">
+        <f>J65/6</f>
+        <v>6.1464982148350389</v>
+      </c>
+      <c r="L65" s="3">
+        <f>(K65-6)/5</f>
+        <v>2.9299642967007777E-2</v>
+      </c>
+      <c r="M65" s="3">
+        <f>L65/1.24</f>
+        <v>2.3628744328232077E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A67" s="3">
+        <f>E6*1.24+E7*0.58+E8*1.24</f>
+        <v>1.1878695652173912</v>
+      </c>
+      <c r="B67" s="3">
+        <f>L27*E6+I42*E7+L65*E8</f>
+        <v>2.6350369765900963E-2</v>
+      </c>
+      <c r="C67" s="3">
+        <f>B67/A67</f>
+        <v>2.2182881469042941E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B70" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+    </row>
+    <row r="71" spans="1:13" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A71" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A72" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" s="15">
+        <f>H21</f>
+        <v>0.27737594649359354</v>
+      </c>
+      <c r="C72" s="15">
+        <f>E39</f>
+        <v>0.12218196457326892</v>
+      </c>
+      <c r="D72" s="15">
+        <f>H59</f>
+        <v>3.3405366386780107E-2</v>
+      </c>
+      <c r="E72" s="15">
+        <f t="array" ref="E72:E77">MMULT(B72:D77,E6:E8)</f>
         <v>7.5421905563212224E-2</v>
       </c>
-      <c r="T8" s="3">
-        <f>RANK(S8,$S$8:$S$13)</f>
+      <c r="F72" s="16">
+        <f>RANK(E72,$E$72:$E$77)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="E9" s="3">
-        <f>SUM(E6:E8)</f>
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="G9" s="3">
-        <f>SUM(G6:G8)</f>
-        <v>9.0276827185242254</v>
-      </c>
-      <c r="H9" s="12">
-        <f>G9/3</f>
-        <v>3.0092275728414086</v>
-      </c>
-      <c r="I9" s="12">
-        <f>(H9-3)/2</f>
-        <v>4.6137864207043133E-3</v>
-      </c>
-      <c r="J9" s="12">
-        <f>I9/0.58</f>
-        <v>7.9548041736281268E-3</v>
-      </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="12">
-        <f t="shared" ref="P9:P13" si="3">H22</f>
+    <row r="73" spans="1:13" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A73" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73" s="15">
+        <f>H22</f>
         <v>0.47514816338345756</v>
       </c>
-      <c r="Q9" s="12">
+      <c r="C73" s="15">
         <f>E40</f>
         <v>0.2298711755233494</v>
       </c>
-      <c r="R9" s="12">
-        <f t="shared" ref="R9:R13" si="4">H60</f>
+      <c r="D73" s="15">
+        <f>H60</f>
         <v>0.1624516557469915</v>
       </c>
-      <c r="S9" s="12">
+      <c r="E73" s="15">
         <v>0.2126419718105011</v>
       </c>
-      <c r="T9" s="3">
-        <f t="shared" ref="T9:T13" si="5">RANK(S9,$S$8:$S$13)</f>
+      <c r="F73" s="16">
+        <f>RANK(E73,$E$72:$E$77)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="H10" s="12"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="12">
-        <f t="shared" si="3"/>
+    <row r="74" spans="1:13" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A74" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B74" s="15">
+        <f>H23</f>
         <v>5.4332795019069527E-2</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="C74" s="16">
         <v>0</v>
       </c>
-      <c r="R10" s="12">
-        <f t="shared" si="4"/>
+      <c r="D74" s="15">
+        <f>H61</f>
         <v>3.984163908796487E-2</v>
       </c>
-      <c r="S10" s="12">
+      <c r="E74" s="15">
         <v>3.8773892866059465E-2</v>
       </c>
-      <c r="T10" s="3">
-        <f t="shared" si="5"/>
+      <c r="F74" s="16">
+        <f>RANK(E74,$E$72:$E$77)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A11" s="3" t="s">
+    <row r="75" spans="1:13" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A75" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75" s="15">
+        <f>H24</f>
+        <v>6.2195484254307778E-2</v>
+      </c>
+      <c r="C75" s="16">
+        <v>0</v>
+      </c>
+      <c r="D75" s="15">
+        <f>H62</f>
+        <v>0.16431335787465107</v>
+      </c>
+      <c r="E75" s="15">
+        <v>0.13668328904482138</v>
+      </c>
+      <c r="F75" s="16">
+        <f>RANK(E75,$E$72:$E$77)</f>
         <v>4</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="12">
-        <f t="shared" si="3"/>
-        <v>6.2195484254307778E-2</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>0</v>
-      </c>
-      <c r="R11" s="12">
-        <f t="shared" si="4"/>
-        <v>0.16431335787465107</v>
-      </c>
-      <c r="S11" s="12">
-        <v>0.13668328904482138</v>
-      </c>
-      <c r="T11" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O12" s="10"/>
-      <c r="P12" s="12">
-        <f t="shared" si="3"/>
+    </row>
+    <row r="76" spans="1:13" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A76" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" s="15">
+        <f>H25</f>
         <v>9.7625703998253016E-2</v>
       </c>
-      <c r="Q12" s="12">
+      <c r="C76" s="15">
         <f>E41</f>
         <v>0.64794685990338152</v>
       </c>
-      <c r="R12" s="12">
-        <f t="shared" si="4"/>
+      <c r="D76" s="15">
+        <f>H63</f>
         <v>0.35283289635998394</v>
       </c>
-      <c r="S12" s="12">
+      <c r="E76" s="15">
         <v>0.33952593834448219</v>
       </c>
-      <c r="T12" s="3">
-        <f t="shared" si="5"/>
+      <c r="F76" s="16">
+        <f>RANK(E76,$E$72:$E$77)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="H13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O13" s="11"/>
-      <c r="P13" s="12">
-        <f t="shared" si="3"/>
+    <row r="77" spans="1:13" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A77" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" s="15">
+        <f>H26</f>
         <v>3.3321906851318611E-2</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="C77" s="16">
         <v>0</v>
       </c>
-      <c r="R13" s="12">
-        <f t="shared" si="4"/>
+      <c r="D77" s="15">
+        <f>H64</f>
         <v>0.24715508454362833</v>
       </c>
-      <c r="S13" s="12">
+      <c r="E77" s="15">
         <v>0.19695300237092336</v>
       </c>
-      <c r="T13" s="3">
-        <f t="shared" si="5"/>
+      <c r="F77" s="16">
+        <f>RANK(E77,$E$72:$E$77)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="14">
-        <v>6</v>
-      </c>
-      <c r="E14" s="14">
-        <v>5</v>
-      </c>
-      <c r="F14" s="14">
-        <v>3</v>
-      </c>
-      <c r="G14" s="14">
-        <v>8</v>
-      </c>
-      <c r="H14" s="12">
-        <f>H21</f>
-        <v>0.27737594649359354</v>
-      </c>
-      <c r="S14" s="3">
-        <f>SUM(S8:S13)</f>
-        <v>0.99999999999999978</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="B15" s="14">
-        <f>1/C14</f>
-        <v>2</v>
-      </c>
-      <c r="C15" s="14">
-        <v>1</v>
-      </c>
-      <c r="D15" s="14">
-        <v>9</v>
-      </c>
-      <c r="E15" s="14">
-        <v>9</v>
-      </c>
-      <c r="F15" s="14">
-        <v>6</v>
-      </c>
-      <c r="G15" s="14">
-        <v>9</v>
-      </c>
-      <c r="H15" s="12">
-        <f t="shared" ref="H15:H19" si="6">H22</f>
-        <v>0.47514816338345756</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="B16" s="14">
-        <f>1/D14</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C16" s="14">
-        <f>1/D15</f>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="D16" s="14">
-        <v>1</v>
-      </c>
-      <c r="E16" s="14">
-        <v>1</v>
-      </c>
-      <c r="F16" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="G16" s="14">
-        <v>2</v>
-      </c>
-      <c r="H16" s="12">
-        <f t="shared" si="6"/>
-        <v>5.4332795019069527E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="14">
-        <f>1/E14</f>
-        <v>0.2</v>
-      </c>
-      <c r="C17" s="14">
-        <f>1/E15</f>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="D17" s="14">
-        <f>1/E16</f>
-        <v>1</v>
-      </c>
-      <c r="E17" s="14">
-        <v>1</v>
-      </c>
-      <c r="F17" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="G17" s="14">
-        <v>3</v>
-      </c>
-      <c r="H17" s="12">
-        <f t="shared" si="6"/>
-        <v>6.2195484254307778E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="14">
-        <f>1/F14</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C18" s="14">
-        <f>1/F15</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D18" s="14">
-        <f>1/F16</f>
-        <v>2</v>
-      </c>
-      <c r="E18" s="14">
-        <f>1/F17</f>
-        <v>2</v>
-      </c>
-      <c r="F18" s="14">
-        <v>1</v>
-      </c>
-      <c r="G18" s="14">
-        <v>3</v>
-      </c>
-      <c r="H18" s="12">
-        <f t="shared" si="6"/>
-        <v>9.7625703998253016E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B19" s="14">
-        <f>1/G14</f>
-        <v>0.125</v>
-      </c>
-      <c r="C19" s="14">
-        <f>1/G15</f>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="D19" s="14">
-        <f>1/G16</f>
-        <v>0.5</v>
-      </c>
-      <c r="E19" s="14">
-        <f>1/G17</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F19" s="14">
-        <f>1/G18</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G19" s="14">
-        <v>1</v>
-      </c>
-      <c r="H19" s="12">
-        <f t="shared" si="6"/>
-        <v>3.3321906851318611E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B20" s="3">
-        <f t="shared" ref="B20:G20" si="7">SUM(B14:B19)</f>
-        <v>3.8250000000000002</v>
-      </c>
-      <c r="C20" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="D20" s="3">
-        <f t="shared" si="7"/>
-        <v>19.5</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" si="7"/>
-        <v>18.333333333333332</v>
-      </c>
-      <c r="F20" s="3">
-        <f t="shared" si="7"/>
-        <v>11.333333333333334</v>
-      </c>
-      <c r="G20" s="3">
-        <f t="shared" si="7"/>
-        <v>26</v>
-      </c>
-      <c r="H20" s="3">
-        <f t="shared" ref="H20:H26" si="8">1/6*SUM(B20:G20)</f>
-        <v>13.498611111111112</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B21" s="3">
-        <f t="shared" ref="B21:G21" si="9">B14/B20</f>
-        <v>0.26143790849673204</v>
-      </c>
-      <c r="C21" s="3">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="9"/>
-        <v>0.30769230769230771</v>
-      </c>
-      <c r="E21" s="3">
-        <f t="shared" si="9"/>
-        <v>0.27272727272727276</v>
-      </c>
-      <c r="F21" s="3">
-        <f t="shared" si="9"/>
-        <v>0.26470588235294118</v>
-      </c>
-      <c r="G21" s="3">
-        <f t="shared" si="9"/>
-        <v>0.30769230769230771</v>
-      </c>
-      <c r="H21" s="12">
-        <f t="shared" si="8"/>
-        <v>0.27737594649359354</v>
-      </c>
-      <c r="I21" s="12">
-        <f t="array" ref="I21:I26">MMULT(B14:G19,H21:H26)</f>
-        <v>1.7113765863765864</v>
-      </c>
-      <c r="J21" s="3">
-        <f>I21/H21</f>
-        <v>6.1698810153176478</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="3">
-        <f t="shared" ref="B22:G22" si="10">B15/B20</f>
-        <v>0.52287581699346408</v>
-      </c>
-      <c r="C22" s="3">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="D22" s="3">
-        <f t="shared" si="10"/>
-        <v>0.46153846153846156</v>
-      </c>
-      <c r="E22" s="3">
-        <f t="shared" si="10"/>
-        <v>0.49090909090909096</v>
-      </c>
-      <c r="F22" s="3">
-        <f t="shared" si="10"/>
-        <v>0.52941176470588236</v>
-      </c>
-      <c r="G22" s="3">
-        <f t="shared" si="10"/>
-        <v>0.34615384615384615</v>
-      </c>
-      <c r="H22" s="12">
-        <f t="shared" si="8"/>
-        <v>0.47514816338345756</v>
-      </c>
-      <c r="I22" s="12">
-        <v>2.964305955482426</v>
-      </c>
-      <c r="J22" s="3">
-        <f t="shared" ref="J22:J26" si="11">I22/H22</f>
-        <v>6.2386981239158237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B23" s="3">
-        <f t="shared" ref="B23:G23" si="12">B16/B20</f>
-        <v>4.3572984749455333E-2</v>
-      </c>
-      <c r="C23" s="3">
-        <f t="shared" si="12"/>
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="D23" s="3">
-        <f t="shared" si="12"/>
-        <v>5.128205128205128E-2</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="shared" si="12"/>
-        <v>5.454545454545455E-2</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="12"/>
-        <v>4.4117647058823525E-2</v>
-      </c>
-      <c r="G23" s="3">
-        <f t="shared" si="12"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-      <c r="H23" s="12">
-        <f t="shared" si="8"/>
-        <v>5.4332795019069527E-2</v>
-      </c>
-      <c r="I23" s="12">
-        <v>0.33100850976667967</v>
-      </c>
-      <c r="J23" s="3">
-        <f t="shared" si="11"/>
-        <v>6.092241520991208</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B24" s="3">
-        <f t="shared" ref="B24:G24" si="13">B17/B20</f>
-        <v>5.2287581699346407E-2</v>
-      </c>
-      <c r="C24" s="3">
-        <f t="shared" si="13"/>
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="D24" s="3">
-        <f t="shared" si="13"/>
-        <v>5.128205128205128E-2</v>
-      </c>
-      <c r="E24" s="3">
-        <f t="shared" si="13"/>
-        <v>5.454545454545455E-2</v>
-      </c>
-      <c r="F24" s="3">
-        <f t="shared" si="13"/>
-        <v>4.4117647058823525E-2</v>
-      </c>
-      <c r="G24" s="3">
-        <f t="shared" si="13"/>
-        <v>0.11538461538461539</v>
-      </c>
-      <c r="H24" s="12">
-        <f t="shared" si="8"/>
-        <v>6.2195484254307778E-2</v>
-      </c>
-      <c r="I24" s="12">
-        <v>0.3735762815011181</v>
-      </c>
-      <c r="J24" s="3">
-        <f t="shared" si="11"/>
-        <v>6.0064856151553077</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B25" s="3">
-        <f t="shared" ref="B25:G25" si="14">B18/B20</f>
-        <v>8.7145969498910666E-2</v>
-      </c>
-      <c r="C25" s="3">
-        <f t="shared" si="14"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D25" s="3">
-        <f t="shared" si="14"/>
-        <v>0.10256410256410256</v>
-      </c>
-      <c r="E25" s="3">
-        <f t="shared" si="14"/>
-        <v>0.1090909090909091</v>
-      </c>
-      <c r="F25" s="3">
-        <f t="shared" si="14"/>
-        <v>8.8235294117647051E-2</v>
-      </c>
-      <c r="G25" s="3">
-        <f t="shared" si="14"/>
-        <v>0.11538461538461539</v>
-      </c>
-      <c r="H25" s="12">
-        <f t="shared" si="8"/>
-        <v>9.7625703998253016E-2</v>
-      </c>
-      <c r="I25" s="12">
-        <v>0.60229799249407079</v>
-      </c>
-      <c r="J25" s="3">
-        <f t="shared" si="11"/>
-        <v>6.1694611954332101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="3">
-        <f t="shared" ref="B26:G26" si="15">B19/B20</f>
-        <v>3.2679738562091505E-2</v>
-      </c>
-      <c r="C26" s="3">
-        <f t="shared" si="15"/>
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="D26" s="3">
-        <f t="shared" si="15"/>
-        <v>2.564102564102564E-2</v>
-      </c>
-      <c r="E26" s="3">
-        <f t="shared" si="15"/>
-        <v>1.8181818181818181E-2</v>
-      </c>
-      <c r="F26" s="3">
-        <f t="shared" si="15"/>
-        <v>2.9411764705882349E-2</v>
-      </c>
-      <c r="G26" s="3">
-        <f t="shared" si="15"/>
-        <v>3.8461538461538464E-2</v>
-      </c>
-      <c r="H26" s="12">
-        <f t="shared" si="8"/>
-        <v>3.3321906851318611E-2</v>
-      </c>
-      <c r="I26" s="12">
-        <v>0.20122826746601255</v>
-      </c>
-      <c r="J26" s="3">
-        <f t="shared" si="11"/>
-        <v>6.038918131662971</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="H27" s="3">
-        <f>SUM(H21:H26)</f>
-        <v>1</v>
-      </c>
-      <c r="J27" s="3">
-        <f>SUM(J21:J26)</f>
-        <v>36.715685602476171</v>
-      </c>
-      <c r="K27" s="12">
-        <f>J27/6</f>
-        <v>6.1192809337460288</v>
-      </c>
-      <c r="L27" s="12">
-        <f>(K27-6)/5</f>
-        <v>2.3856186749205754E-2</v>
-      </c>
-      <c r="M27" s="12">
-        <f>L27/1.24</f>
-        <v>1.9238860281617545E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A29" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A30" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D33" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="E33" s="12">
-        <f>E39</f>
-        <v>0.12218196457326892</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B34" s="3">
-        <f>1/C33</f>
-        <v>2</v>
-      </c>
-      <c r="C34" s="3">
-        <v>1</v>
-      </c>
-      <c r="D34" s="3">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E34" s="12">
-        <f t="shared" ref="E34:E35" si="16">E40</f>
-        <v>0.2298711755233494</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B35" s="3">
-        <f>1/D33</f>
-        <v>5</v>
-      </c>
-      <c r="C35" s="3">
-        <f>1/D34</f>
-        <v>3</v>
-      </c>
-      <c r="D35" s="3">
-        <v>1</v>
-      </c>
-      <c r="E35" s="12">
-        <f t="shared" si="16"/>
-        <v>0.64794685990338152</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B36" s="3">
-        <f>SUM(B33:B35)</f>
-        <v>8</v>
-      </c>
-      <c r="C36" s="3">
-        <f>SUM(C33:C35)</f>
-        <v>4.5</v>
-      </c>
-      <c r="D36" s="3">
-        <f>SUM(D33:D35)</f>
-        <v>1.5333333333333332</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B37" s="3">
-        <f>B36</f>
-        <v>8</v>
-      </c>
-      <c r="C37" s="3">
-        <f t="shared" ref="C37:D37" si="17">C36</f>
-        <v>4.5</v>
-      </c>
-      <c r="D37" s="3">
-        <f t="shared" si="17"/>
-        <v>1.5333333333333332</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B38" s="3">
-        <f>B36</f>
-        <v>8</v>
-      </c>
-      <c r="C38" s="3">
-        <f t="shared" ref="C38:D38" si="18">C36</f>
-        <v>4.5</v>
-      </c>
-      <c r="D38" s="3">
-        <f t="shared" si="18"/>
-        <v>1.5333333333333332</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B39" s="3">
-        <f>B33/B36</f>
-        <v>0.125</v>
-      </c>
-      <c r="C39" s="3">
-        <f>C33/C36</f>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="D39" s="3">
-        <f>D33/D36</f>
-        <v>0.13043478260869568</v>
-      </c>
-      <c r="E39" s="12">
-        <f>1/3*SUM(B39:D39)</f>
-        <v>0.12218196457326892</v>
-      </c>
-      <c r="F39" s="12">
-        <f t="array" ref="F39:F41">MMULT(B33:D35,E39:E41)</f>
-        <v>0.36670692431561991</v>
-      </c>
-      <c r="G39" s="3">
-        <f>F39/E39</f>
-        <v>3.0013179571663917</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B40" s="3">
-        <f t="shared" ref="B40:D40" si="19">B34/B37</f>
-        <v>0.25</v>
-      </c>
-      <c r="C40" s="3">
-        <f t="shared" si="19"/>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="D40" s="3">
-        <f t="shared" si="19"/>
-        <v>0.21739130434782608</v>
-      </c>
-      <c r="E40" s="12">
-        <f t="shared" ref="E40:E41" si="20">1/3*SUM(B40:D40)</f>
-        <v>0.2298711755233494</v>
-      </c>
-      <c r="F40" s="12">
-        <v>0.69021739130434778</v>
-      </c>
-      <c r="G40" s="3">
-        <f t="shared" ref="G40:G41" si="21">F40/E40</f>
-        <v>3.0026269702276709</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B41" s="3">
-        <f t="shared" ref="B41:D41" si="22">B35/B38</f>
-        <v>0.625</v>
-      </c>
-      <c r="C41" s="3">
-        <f t="shared" si="22"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D41" s="3">
-        <f t="shared" si="22"/>
-        <v>0.65217391304347827</v>
-      </c>
-      <c r="E41" s="12">
-        <f t="shared" si="20"/>
-        <v>0.64794685990338152</v>
-      </c>
-      <c r="F41" s="12">
-        <v>1.9484702093397743</v>
-      </c>
-      <c r="G41" s="3">
-        <f t="shared" si="21"/>
-        <v>3.0071450761105933</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="E42" s="3">
-        <f>SUM(E39:E41)</f>
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="G42" s="3">
-        <f>SUM(G39:G41)</f>
-        <v>9.0110900035046555</v>
-      </c>
-      <c r="H42" s="12">
-        <f>G42/3</f>
-        <v>3.0036966678348853</v>
-      </c>
-      <c r="I42" s="12">
-        <f>(H42-3)/2</f>
-        <v>1.8483339174426572E-3</v>
-      </c>
-      <c r="J42" s="12">
-        <f>I42/0.58</f>
-        <v>3.1867826162804438E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A44" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A45" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B47" s="3">
-        <v>1</v>
-      </c>
-      <c r="C47" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="D47" s="3">
-        <v>1</v>
-      </c>
-      <c r="E47" s="3">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F47" s="3">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="G47" s="3">
-        <v>0.125</v>
-      </c>
-      <c r="H47" s="12">
-        <f>H59</f>
-        <v>3.3405366386780107E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B48" s="3">
-        <f>1/C47</f>
-        <v>5</v>
-      </c>
-      <c r="C48" s="3">
-        <v>1</v>
-      </c>
-      <c r="D48" s="3">
-        <v>5</v>
-      </c>
-      <c r="E48" s="3">
-        <v>1</v>
-      </c>
-      <c r="F48" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G48" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H48" s="12">
-        <f t="shared" ref="H48:H52" si="23">H60</f>
-        <v>0.1624516557469915</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B49" s="3">
-        <f>1/D47</f>
-        <v>1</v>
-      </c>
-      <c r="C49" s="3">
-        <f>1/D48</f>
-        <v>0.2</v>
-      </c>
-      <c r="D49" s="3">
-        <v>1</v>
-      </c>
-      <c r="E49" s="3">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F49" s="3">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G49" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="H49" s="12">
-        <f t="shared" si="23"/>
-        <v>3.984163908796487E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B50" s="3">
-        <f>1/E47</f>
-        <v>6</v>
-      </c>
-      <c r="C50" s="3">
-        <f>1/E48</f>
-        <v>1</v>
-      </c>
-      <c r="D50" s="3">
-        <f>1/E49</f>
-        <v>6</v>
-      </c>
-      <c r="E50" s="3">
-        <v>1</v>
-      </c>
-      <c r="F50" s="3">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G50" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H50" s="12">
-        <f t="shared" si="23"/>
-        <v>0.16431335787465107</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B51" s="3">
-        <f>1/F47</f>
-        <v>9</v>
-      </c>
-      <c r="C51" s="3">
-        <f>1/F48</f>
-        <v>2</v>
-      </c>
-      <c r="D51" s="3">
-        <f>1/F49</f>
-        <v>6</v>
-      </c>
-      <c r="E51" s="3">
-        <f>1/F50</f>
-        <v>3</v>
-      </c>
-      <c r="F51" s="3">
-        <v>1</v>
-      </c>
-      <c r="G51" s="3">
-        <v>2</v>
-      </c>
-      <c r="H51" s="12">
-        <f t="shared" si="23"/>
-        <v>0.35283289635998394</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B52" s="3">
-        <f>1/G47</f>
-        <v>8</v>
-      </c>
-      <c r="C52" s="3">
-        <f>1/G48</f>
-        <v>2</v>
-      </c>
-      <c r="D52" s="3">
-        <f>1/G49</f>
-        <v>5</v>
-      </c>
-      <c r="E52" s="3">
-        <f>1/G50</f>
-        <v>2</v>
-      </c>
-      <c r="F52" s="3">
-        <f>1/G51</f>
-        <v>0.5</v>
-      </c>
-      <c r="G52" s="3">
-        <v>1</v>
-      </c>
-      <c r="H52" s="12">
-        <f t="shared" si="23"/>
-        <v>0.24715508454362833</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B53" s="3">
-        <f>SUM(B47:B52)</f>
-        <v>30</v>
-      </c>
-      <c r="C53" s="3">
-        <f t="shared" ref="C53:G53" si="24">SUM(C47:C52)</f>
-        <v>6.4</v>
-      </c>
-      <c r="D53" s="3">
-        <f t="shared" si="24"/>
-        <v>24</v>
-      </c>
-      <c r="E53" s="3">
-        <f t="shared" si="24"/>
-        <v>7.3333333333333339</v>
-      </c>
-      <c r="F53" s="3">
-        <f t="shared" si="24"/>
-        <v>2.6111111111111112</v>
-      </c>
-      <c r="G53" s="3">
-        <f t="shared" si="24"/>
-        <v>4.3250000000000002</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B54" s="3">
-        <f>B53</f>
-        <v>30</v>
-      </c>
-      <c r="C54" s="3">
-        <f t="shared" ref="C54:G54" si="25">C53</f>
-        <v>6.4</v>
-      </c>
-      <c r="D54" s="3">
-        <f t="shared" si="25"/>
-        <v>24</v>
-      </c>
-      <c r="E54" s="3">
-        <f t="shared" si="25"/>
-        <v>7.3333333333333339</v>
-      </c>
-      <c r="F54" s="3">
-        <f t="shared" si="25"/>
-        <v>2.6111111111111112</v>
-      </c>
-      <c r="G54" s="3">
-        <f t="shared" si="25"/>
-        <v>4.3250000000000002</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B55" s="3">
-        <f>B53</f>
-        <v>30</v>
-      </c>
-      <c r="C55" s="3">
-        <f t="shared" ref="C55:G55" si="26">C53</f>
-        <v>6.4</v>
-      </c>
-      <c r="D55" s="3">
-        <f t="shared" si="26"/>
-        <v>24</v>
-      </c>
-      <c r="E55" s="3">
-        <f t="shared" si="26"/>
-        <v>7.3333333333333339</v>
-      </c>
-      <c r="F55" s="3">
-        <f t="shared" si="26"/>
-        <v>2.6111111111111112</v>
-      </c>
-      <c r="G55" s="3">
-        <f t="shared" si="26"/>
-        <v>4.3250000000000002</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B56" s="3">
-        <f>B53</f>
-        <v>30</v>
-      </c>
-      <c r="C56" s="3">
-        <f t="shared" ref="C56:G56" si="27">C53</f>
-        <v>6.4</v>
-      </c>
-      <c r="D56" s="3">
-        <f t="shared" si="27"/>
-        <v>24</v>
-      </c>
-      <c r="E56" s="3">
-        <f t="shared" si="27"/>
-        <v>7.3333333333333339</v>
-      </c>
-      <c r="F56" s="3">
-        <f t="shared" si="27"/>
-        <v>2.6111111111111112</v>
-      </c>
-      <c r="G56" s="3">
-        <f t="shared" si="27"/>
-        <v>4.3250000000000002</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B57" s="3">
-        <f>B53</f>
-        <v>30</v>
-      </c>
-      <c r="C57" s="3">
-        <f t="shared" ref="C57:G57" si="28">C53</f>
-        <v>6.4</v>
-      </c>
-      <c r="D57" s="3">
-        <f t="shared" si="28"/>
-        <v>24</v>
-      </c>
-      <c r="E57" s="3">
-        <f t="shared" si="28"/>
-        <v>7.3333333333333339</v>
-      </c>
-      <c r="F57" s="3">
-        <f t="shared" si="28"/>
-        <v>2.6111111111111112</v>
-      </c>
-      <c r="G57" s="3">
-        <f t="shared" si="28"/>
-        <v>4.3250000000000002</v>
-      </c>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B58" s="3">
-        <f>B53</f>
-        <v>30</v>
-      </c>
-      <c r="C58" s="3">
-        <f t="shared" ref="C58:G58" si="29">C53</f>
-        <v>6.4</v>
-      </c>
-      <c r="D58" s="3">
-        <f t="shared" si="29"/>
-        <v>24</v>
-      </c>
-      <c r="E58" s="3">
-        <f t="shared" si="29"/>
-        <v>7.3333333333333339</v>
-      </c>
-      <c r="F58" s="3">
-        <f t="shared" si="29"/>
-        <v>2.6111111111111112</v>
-      </c>
-      <c r="G58" s="3">
-        <f t="shared" si="29"/>
-        <v>4.3250000000000002</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B59" s="3">
-        <f>B47/B53</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="C59" s="3">
-        <f t="shared" ref="C59:G59" si="30">C47/C53</f>
-        <v>3.125E-2</v>
-      </c>
-      <c r="D59" s="3">
-        <f t="shared" si="30"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E59" s="3">
-        <f t="shared" si="30"/>
-        <v>2.2727272727272724E-2</v>
-      </c>
-      <c r="F59" s="3">
-        <f t="shared" si="30"/>
-        <v>4.2553191489361701E-2</v>
-      </c>
-      <c r="G59" s="3">
-        <f t="shared" si="30"/>
-        <v>2.8901734104046242E-2</v>
-      </c>
-      <c r="H59" s="12">
-        <f>1/6*SUM(B59:G59)</f>
-        <v>3.3405366386780107E-2</v>
-      </c>
-      <c r="I59" s="12">
-        <f t="array" ref="I59:I64">MMULT(B47:G52,H59:H64)</f>
-        <v>0.20322093698898133</v>
-      </c>
-      <c r="J59" s="3">
-        <f>I59/H59</f>
-        <v>6.0834817566738115</v>
-      </c>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B60" s="3">
-        <f t="shared" ref="B60:G60" si="31">B48/B54</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C60" s="3">
-        <f t="shared" si="31"/>
-        <v>0.15625</v>
-      </c>
-      <c r="D60" s="3">
-        <f t="shared" si="31"/>
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="E60" s="3">
-        <f t="shared" si="31"/>
-        <v>0.13636363636363635</v>
-      </c>
-      <c r="F60" s="3">
-        <f t="shared" si="31"/>
-        <v>0.19148936170212766</v>
-      </c>
-      <c r="G60" s="3">
-        <f t="shared" si="31"/>
-        <v>0.11560693641618497</v>
-      </c>
-      <c r="H60" s="12">
-        <f t="shared" ref="H60:H64" si="32">1/6*SUM(B60:G60)</f>
-        <v>0.1624516557469915</v>
-      </c>
-      <c r="I60" s="12">
-        <v>0.99299403144717369</v>
-      </c>
-      <c r="J60" s="3">
-        <f t="shared" ref="J60:J64" si="33">I60/H60</f>
-        <v>6.1125510040581004</v>
-      </c>
-    </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B61" s="3">
-        <f t="shared" ref="B61:G61" si="34">B49/B55</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="C61" s="3">
-        <f t="shared" si="34"/>
-        <v>3.125E-2</v>
-      </c>
-      <c r="D61" s="3">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E61" s="3">
-        <f t="shared" si="34"/>
-        <v>2.2727272727272724E-2</v>
-      </c>
-      <c r="F61" s="3">
-        <f t="shared" si="34"/>
-        <v>6.3829787234042548E-2</v>
-      </c>
-      <c r="G61" s="3">
-        <f t="shared" si="34"/>
-        <v>4.6242774566473986E-2</v>
-      </c>
-      <c r="H61" s="12">
-        <f t="shared" si="32"/>
-        <v>3.984163908796487E-2</v>
-      </c>
-      <c r="I61" s="12">
-        <v>0.24135939590530811</v>
-      </c>
-      <c r="J61" s="3">
-        <f t="shared" si="33"/>
-        <v>6.0579685331825752</v>
-      </c>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B62" s="3">
-        <f t="shared" ref="B62:G62" si="35">B50/B56</f>
-        <v>0.2</v>
-      </c>
-      <c r="C62" s="3">
-        <f t="shared" si="35"/>
-        <v>0.15625</v>
-      </c>
-      <c r="D62" s="3">
-        <f t="shared" si="35"/>
-        <v>0.25</v>
-      </c>
-      <c r="E62" s="3">
-        <f t="shared" si="35"/>
-        <v>0.13636363636363635</v>
-      </c>
-      <c r="F62" s="3">
-        <f t="shared" si="35"/>
-        <v>0.1276595744680851</v>
-      </c>
-      <c r="G62" s="3">
-        <f t="shared" si="35"/>
-        <v>0.11560693641618497</v>
-      </c>
-      <c r="H62" s="12">
-        <f t="shared" si="32"/>
-        <v>0.16431335787465107</v>
-      </c>
-      <c r="I62" s="12">
-        <v>1.0074355541952547</v>
-      </c>
-      <c r="J62" s="3">
-        <f t="shared" si="33"/>
-        <v>6.1311847510522677</v>
-      </c>
-    </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B63" s="3">
-        <f t="shared" ref="B63:G63" si="36">B51/B57</f>
-        <v>0.3</v>
-      </c>
-      <c r="C63" s="3">
-        <f t="shared" si="36"/>
-        <v>0.3125</v>
-      </c>
-      <c r="D63" s="3">
-        <f t="shared" si="36"/>
-        <v>0.25</v>
-      </c>
-      <c r="E63" s="3">
-        <f t="shared" si="36"/>
-        <v>0.40909090909090906</v>
-      </c>
-      <c r="F63" s="3">
-        <f t="shared" si="36"/>
-        <v>0.38297872340425532</v>
-      </c>
-      <c r="G63" s="3">
-        <f t="shared" si="36"/>
-        <v>0.46242774566473988</v>
-      </c>
-      <c r="H63" s="12">
-        <f t="shared" si="32"/>
-        <v>0.35283289635998394</v>
-      </c>
-      <c r="I63" s="12">
-        <v>2.2046845825739867</v>
-      </c>
-      <c r="J63" s="3">
-        <f t="shared" si="33"/>
-        <v>6.2485233245502672</v>
-      </c>
-    </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B64" s="3">
-        <f t="shared" ref="B64:G64" si="37">B52/B58</f>
-        <v>0.26666666666666666</v>
-      </c>
-      <c r="C64" s="3">
-        <f t="shared" si="37"/>
-        <v>0.3125</v>
-      </c>
-      <c r="D64" s="3">
-        <f t="shared" si="37"/>
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="E64" s="3">
-        <f t="shared" si="37"/>
-        <v>0.27272727272727271</v>
-      </c>
-      <c r="F64" s="3">
-        <f t="shared" si="37"/>
-        <v>0.19148936170212766</v>
-      </c>
-      <c r="G64" s="3">
-        <f t="shared" si="37"/>
-        <v>0.23121387283236994</v>
-      </c>
-      <c r="H64" s="12">
-        <f t="shared" si="32"/>
-        <v>0.24715508454362833</v>
-      </c>
-      <c r="I64" s="12">
-        <v>1.5435526865009705</v>
-      </c>
-      <c r="J64" s="3">
-        <f t="shared" si="33"/>
-        <v>6.2452799194932176</v>
-      </c>
-      <c r="K64" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L64" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M64" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="8:13" x14ac:dyDescent="0.15">
-      <c r="H65" s="3">
-        <f>SUM(H59:H64)</f>
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="J65" s="3">
-        <f>SUM(J59:J64)</f>
-        <v>36.878989289010235</v>
-      </c>
-      <c r="K65" s="12">
-        <f>J65/6</f>
-        <v>6.1464982148350389</v>
-      </c>
-      <c r="L65" s="12">
-        <f>(K65-6)/5</f>
-        <v>2.9299642967007777E-2</v>
-      </c>
-      <c r="M65" s="12">
-        <f>L65/1.24</f>
-        <v>2.3628744328232077E-2</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -5638,122 +5029,122 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A1" s="13">
+      <c r="A1" s="4">
         <v>1</v>
       </c>
-      <c r="B1" s="13">
+      <c r="B1" s="4">
         <v>0.5</v>
       </c>
-      <c r="C1" s="13">
+      <c r="C1" s="4">
         <v>6</v>
       </c>
-      <c r="D1" s="13">
+      <c r="D1" s="4">
         <v>5</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E1" s="4">
         <v>3</v>
       </c>
-      <c r="F1" s="13">
+      <c r="F1" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A2" s="13">
+      <c r="A2" s="4">
         <v>2</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="4">
         <v>9</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="4">
         <v>9</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="4">
         <v>6</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="4">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A3" s="16">
+      <c r="A3" s="6">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="4">
         <v>0.1111111111111111</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="4">
         <v>0.5</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A4" s="13">
+      <c r="A4" s="4">
         <v>0.2</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="4">
         <v>0.1111111111111111</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="4">
         <v>0.5</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A5" s="13">
+      <c r="A5" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="4">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="4">
         <v>2</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="4">
         <v>2</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A6" s="13">
+      <c r="A6" s="4">
         <v>0.125</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="4">
         <v>0.1111111111111111</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="4">
         <v>0.5</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="4">
         <v>1</v>
       </c>
     </row>
@@ -5761,7 +5152,7 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="7">
         <v>41276</v>
       </c>
       <c r="J11">
@@ -5798,10 +5189,10 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="H13" s="17">
+      <c r="H13" s="7">
         <v>41280</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="7">
         <v>41283</v>
       </c>
       <c r="J13">
@@ -5810,7 +5201,7 @@
       <c r="K13">
         <v>1</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="7">
         <v>41276</v>
       </c>
       <c r="M13">
@@ -5818,10 +5209,10 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="H14" s="17">
+      <c r="H14" s="7">
         <v>41279</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="7">
         <v>41283</v>
       </c>
       <c r="J14">
@@ -5830,7 +5221,7 @@
       <c r="K14">
         <v>1</v>
       </c>
-      <c r="L14" s="17">
+      <c r="L14" s="7">
         <v>41276</v>
       </c>
       <c r="M14">
@@ -5838,10 +5229,10 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="H15" s="17">
+      <c r="H15" s="7">
         <v>41277</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="7">
         <v>41280</v>
       </c>
       <c r="J15">
@@ -5858,19 +5249,19 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="H16" s="17">
+      <c r="H16" s="7">
         <v>41282</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="7">
         <v>41283</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="7">
         <v>41276</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K16" s="7">
         <v>41277</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="7">
         <v>41277</v>
       </c>
       <c r="M16">
@@ -5878,127 +5269,127 @@
       </c>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.15">
-      <c r="E19" s="13">
+      <c r="E19" s="4">
         <v>1</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="4">
         <v>0.5</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="4">
         <v>6</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="4">
         <v>5</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.15">
-      <c r="E20" s="13">
+      <c r="E20" s="4">
         <v>2</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="4">
         <v>1</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="4">
         <v>9</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="4">
         <v>9</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="4">
         <v>6</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="4">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.15">
-      <c r="E21" s="16">
+      <c r="E21" s="6">
         <v>0.16666666666666666</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="4">
         <v>0.1111111111111111</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="4">
         <v>1</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="4">
         <v>1</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="4">
         <v>0.5</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.15">
-      <c r="E22" s="13">
+      <c r="E22" s="4">
         <v>0.2</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="4">
         <v>0.1111111111111111</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="4">
         <v>1</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="4">
         <v>1</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="4">
         <v>0.5</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.15">
-      <c r="E23" s="13">
+      <c r="E23" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="4">
         <v>0.16666666666666666</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="4">
         <v>2</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="4">
         <v>2</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="4">
         <v>1</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.15">
-      <c r="E24" s="13">
+      <c r="E24" s="4">
         <v>0.125</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="4">
         <v>0.1111111111111111</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="4">
         <v>0.5</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6011,7 +5402,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>